<commit_message>
A new as_zapisy file and a corrected version of pr_usos.
</commit_message>
<xml_diff>
--- a/inst/pr_usos.xlsx
+++ b/inst/pr_usos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zajac/Dropbox/PEJK/ASIA/dane do testowania/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zajac/Dropbox/PEJK/ASIA/Pakiet ASIA/ASIA1/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91999E7B-9B5F-FB43-98FA-E1B2B246423B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7973A09-729F-634B-9C39-2BA0661EAE11}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="7020" windowWidth="24640" windowHeight="14600" xr2:uid="{950A28FE-273B-4D41-8814-F629788AEE53}"/>
+    <workbookView xWindow="12020" yWindow="2680" windowWidth="24640" windowHeight="14600" xr2:uid="{950A28FE-273B-4D41-8814-F629788AEE53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8232AB38-F1C4-134C-93F7-8479B20BD550}">
   <dimension ref="A1:OF66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,7 +539,7 @@
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:396" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:396" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -973,7 +973,7 @@
     </row>
     <row r="2" spans="1:396" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>97040200001</v>
+        <v>98090100001</v>
       </c>
       <c r="B2">
         <v>11111</v>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="3" spans="1:396" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>97040200002</v>
+        <v>98090100002</v>
       </c>
       <c r="B3">
         <v>11112</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="4" spans="1:396" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>97040200003</v>
+        <v>98090100003</v>
       </c>
       <c r="B4">
         <v>11113</v>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="5" spans="1:396" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>97040200004</v>
+        <v>98090100004</v>
       </c>
       <c r="B5">
         <v>11114</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="6" spans="1:396" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>97040200005</v>
+        <v>98090100005</v>
       </c>
       <c r="B6">
         <v>11115</v>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="7" spans="1:396" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>97040200006</v>
+        <v>98090100006</v>
       </c>
       <c r="B7">
         <v>11116</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="8" spans="1:396" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>97040200007</v>
+        <v>98090100007</v>
       </c>
       <c r="B8">
         <v>11117</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="9" spans="1:396" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>97040200008</v>
+        <v>98090100008</v>
       </c>
       <c r="B9">
         <v>11118</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="10" spans="1:396" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>97040200009</v>
+        <v>98090100009</v>
       </c>
       <c r="B10">
         <v>11119</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="11" spans="1:396" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>97040200010</v>
+        <v>98090100010</v>
       </c>
       <c r="B11">
         <v>11120</v>

</xml_diff>